<commit_message>
Modifications du design de l'appli : entête et barre d'onglet.
</commit_message>
<xml_diff>
--- a/Modifs_Juliette/Base_de_données.xlsx
+++ b/Modifs_Juliette/Base_de_données.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -499,6 +499,75 @@
         <v>7.237476542487647</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SCHMITT</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Hadrien</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>21 Bd Maréchal Lyautey, 38000 Grenoble</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>45.1859198</v>
+      </c>
+      <c r="E7">
+        <v>5.731540139877457</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SCHMITT</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Hadrien</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>21 Bd Maréchal Lyautey, 38000 Grenoble</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>45.1859198</v>
+      </c>
+      <c r="E8">
+        <v>5.731540139877457</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ASTRID</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Monique</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>30 Rue Rambaud, 17000 La Rochelle</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>46.16360619065998</v>
+      </c>
+      <c r="E9">
+        <v>-1.155014376554859</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>